<commit_message>
add test cases for ansteel/story SDL-8754
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/ansteel-api-engine-test-data.xlsx
+++ b/src/main/resources/test-data-xls/ansteel-api-engine-test-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E374F055-C659-4629-8791-060C671EA1EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCFE71B5-004E-4597-9860-3D063DF34A0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="43">
   <si>
     <t>description</t>
   </si>
@@ -60,20 +60,81 @@
     <t>sqlStatement</t>
   </si>
   <si>
-    <t>databrain-smartspace-test-1</t>
-  </si>
-  <si>
     <t>Successfully</t>
   </si>
   <si>
-    <t>获取过程参数预警列表</t>
-  </si>
-  <si>
     <t>Alarm_Data</t>
   </si>
   <si>
+    <t>获取过程参数预警列表
+condition(_gte,_lte)
+order(`timestamp` ASC)</t>
+  </si>
+  <si>
+    <t>获取过程参数预警列表
+condition(_gte,_lte)
+order(`timestamp` DESC)</t>
+  </si>
+  <si>
+    <t>获取过程参数预警列表
+condition(_gte,_lte)
+order(`timestamp` ASC)
+pageIndex:1
+pageSize:20</t>
+  </si>
+  <si>
+    <t>获取过程参数预警列表
+condition(_eq)
+order(`timestamp` ASC)
+pageIndex:1
+pageSize:20</t>
+  </si>
+  <si>
     <t>{
-  Alarm_Data(cond:"{timestamp:{_gte:\"2022-05-16 16:00:00.000\",_lte:\"2022-05-16 16:01:00.000\"}}", authInfo:"", order:"timestamp asc")
+  Alarm_DataConnection(cond:"{processNum:{_eq:\"FCE\"}}", authInfo:"", order:"timestamp ASC", after:"1", first:20)
+  {
+    totalElements
+    totalPages
+    pageSize
+    page
+    numberOfElements
+    edges {
+      node {
+        cmdPoint
+        timestamp
+        alarmRuleId
+        alarmType
+        sensorId
+        absValue
+        processNum
+        coilNum
+        id
+      }
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>ansteel-function-test-1</t>
+  </si>
+  <si>
+    <t>ansteel-function-test-2</t>
+  </si>
+  <si>
+    <t>ansteel-function-test-3</t>
+  </si>
+  <si>
+    <t>ansteel-function-test-4</t>
+  </si>
+  <si>
+    <t>获取过程参数</t>
+  </si>
+  <si>
+    <t>ansteel-function-test-5</t>
+  </si>
+  <si>
+    <t>{
+  Alarm_Data(cond:"{timestamp:{_gte:\"2022-01-03 07:00:00.000\",_lte:\"2022-01-03 08:00:00.000\"}}", authInfo:"", order:"timestamp ASC")
   {
     cmdPoint
     timestamp
@@ -88,8 +149,148 @@
 }</t>
   </si>
   <si>
-    <t>SELECT cmdPoint ,`timestamp` ,alarmRuleId,alarmType,sensorId,absValue,processNum,coilNum FROM Alarm_Data ad 
-WHERE `timestamp` &gt;= '2022-05-16 16:00:00.000' and `timestamp` &lt;= '2022-05-16 16:01:00.000' order by `timestamp` ASC;</t>
+    <t>{
+  Alarm_Data(cond:"{timestamp:{_gte:\"2022-01-03 07:00:00.000\",_lte:\"2022-01-03 08:00:00.000\"}}", authInfo:"", order:"timestamp DESC")
+  {
+    cmdPoint
+    timestamp
+    alarmRuleId
+    alarmType
+    sensorId
+    absValue
+    processNum
+    coilNum
+    id
+  }
+}</t>
+  </si>
+  <si>
+    <t>{
+  Alarm_DataConnection(cond:"{timestamp:{_gte:\"2022-01-03 07:00:00.000\",_lte:\"2022-01-03 08:00:00.000\"}}", authInfo:"", order:"timestamp ASC", after:"1", first:20)
+  {
+    totalElements
+    totalPages
+    pageSize
+    page
+    numberOfElements
+    edges {
+      node {
+        cmdPoint
+        timestamp
+        alarmRuleId
+        alarmType
+        sensorId
+        absValue
+        processNum
+        coilNum
+        id
+      }
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>Alarm_DataConnection-&gt;edges</t>
+  </si>
+  <si>
+    <t>{
+  Sensor(cond:"{processNum:{_eq:\"FCE\"}}", authInfo:"", order:"")
+  {
+    pass
+    source
+    unit
+    rate
+    processNum
+    coilIdNo
+    internalSensorName
+    frequency
+    pdaAddress
+    physicalMeaning
+    processRange
+    sourceSensorName
+    sensorDescription
+    eventStatus
+    eventTag
+    ifId
+    diffL2L1
+    id
+    device
+    type
+  }
+}</t>
+  </si>
+  <si>
+    <t>获取过程参数数据</t>
+  </si>
+  <si>
+    <t>database</t>
+  </si>
+  <si>
+    <t>chdb</t>
+  </si>
+  <si>
+    <t>SELECT cmdPoint ,`timestamp` ,alarmRuleId,alarmType,sensorId,absValue,processNum,coilNum FROM chdb.Alarm_Data ad 
+WHERE `timestamp` &gt;= '2022-01-03 07:00:00.000' and `timestamp` &lt;= '2022-01-03 08:00:00.000' order by `timestamp` ASC;</t>
+  </si>
+  <si>
+    <t>SELECT cmdPoint ,`timestamp` ,alarmRuleId,alarmType,sensorId,absValue,processNum,coilNum FROM  chdb.Alarm_Data ad 
+WHERE `timestamp` &gt;= '2022-01-03 07:00:00.000' and `timestamp` &lt;= '2022-01-03 08:00:00.000' order by `timestamp` DESC;</t>
+  </si>
+  <si>
+    <t>SELECT cmdPoint ,`timestamp` ,alarmRuleId,alarmType,sensorId,absValue,processNum,coilNum FROM  chdb.Alarm_Data ad 
+WHERE `timestamp` &gt;= '2022-01-03 07:00:00.000' and `timestamp` &lt;= '2022-01-03 08:00:00.000' order by `timestamp` ASC limit 20;</t>
+  </si>
+  <si>
+    <t>SELECT cmdPoint ,`timestamp` ,alarmRuleId,alarmType,sensorId,absValue,processNum,coilNum FROM  chdb.Alarm_Data ad 
+WHERE processNum = 'FCE' order by `timestamp` ASC limit 20;</t>
+  </si>
+  <si>
+    <t>datacleaning</t>
+  </si>
+  <si>
+    <t>datamanagement</t>
+  </si>
+  <si>
+    <t>select pass,source,unit,rate,process as processNum,coil_id_no as coilIdNo,coil_id_no as coilIdNo,internal_sensor_name as internalSensorName,
+freq as frequency,pda_abs_addr as frequency,pda_abs_addr as pdaAddress,multiple_setting as physicalMeaning,process_range as processRange,
+source_sensor_name as sourceSensorName,description as sensorDescription,event_status as eventStatus,event_tag as eventTag,
+if_id as ifId,l2_l1_diff as diffL2L1,internal_sensor_name as id,device,type from public.sensor s where process = 'FCE';</t>
+  </si>
+  <si>
+    <t>获取全产线报警最频繁的过程参数
+condition(_gte,_lte)
+order(`createTime` ASC)</t>
+  </si>
+  <si>
+    <t>{
+  Alarm_TopN(cond:"{createTime:{_gte:\"2022-05-17 00:00:00.000\",_lte:\"2022-05-17 23:59:59.000\"}}", authInfo:"", order:"createTime ASC")
+  {
+    count
+    coilNum
+    sensorId
+    createTime
+    id
+    period
+    periodEndTime
+    periodStartTime
+  }
+}</t>
+  </si>
+  <si>
+    <t>select * from public.datalayer_alarm_topn where create_time &gt;= '2022-05-17 00:00:00.000' 
+and create_time &lt;= '2022-05-17 23:59:59.000' order by create_time asc</t>
+  </si>
+  <si>
+    <t>ansteel-function-test-6</t>
+  </si>
+  <si>
+    <t>ansteel-function-test-7</t>
+  </si>
+  <si>
+    <t>Sensor</t>
+  </si>
+  <si>
+    <t>Alarm_TopN</t>
   </si>
 </sst>
 </file>
@@ -463,26 +664,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13585E94-2A3C-423F-8526-0CA62361FED2}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="53.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="12.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="59.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="56.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -496,42 +698,213 @@
         <v>5</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="220.8">
+    <row r="2" spans="1:9" ht="150" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="5">
+        <v>200</v>
+      </c>
+      <c r="H2" s="5">
+        <v>100000</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="150" customHeight="1">
+      <c r="A3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="C3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="5">
+        <v>200</v>
+      </c>
+      <c r="H3" s="5">
+        <v>100000</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="150" customHeight="1">
+      <c r="A4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="C4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" s="5">
+        <v>200</v>
+      </c>
+      <c r="H4" s="5">
+        <v>100000</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="150" customHeight="1">
+      <c r="A5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="5">
+      <c r="C5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="5">
         <v>200</v>
       </c>
-      <c r="G2" s="5">
+      <c r="H5" s="5">
         <v>100000</v>
       </c>
-      <c r="H2" s="5" t="s">
-        <v>9</v>
+      <c r="I5" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="150" customHeight="1">
+      <c r="A6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" s="5">
+        <v>200</v>
+      </c>
+      <c r="H6" s="5">
+        <v>100000</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="150" customHeight="1">
+      <c r="A7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="G7" s="5">
+        <v>200</v>
+      </c>
+      <c r="H7" s="5">
+        <v>100000</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="150" customHeight="1">
+      <c r="A8" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" s="5">
+        <v>200</v>
+      </c>
+      <c r="H8" s="5">
+        <v>100000</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add test case of sdl-8818
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/ansteel-api-engine-test-data.xlsx
+++ b/src/main/resources/test-data-xls/ansteel-api-engine-test-data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\data-layer-automation\src\main\resources\test-data-xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\auto_worksapce\feature-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCFE71B5-004E-4597-9860-3D063DF34A0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8C4CDAC-9434-494B-B710-82759642D399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="64">
   <si>
     <t>description</t>
   </si>
@@ -292,36 +292,182 @@
   <si>
     <t>Alarm_TopN</t>
   </si>
+  <si>
+    <t>ansteel-function-test-8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">获取在生产的钢卷condition(_eq)
+order(`timestamp` ASC)	</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coil</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+  Coil(cond:"{coilStatus:{_eq:\"true\"}}", authInfo:"", order:"")
+  {
+    coilNum 
+    coilStatus 
+    coilWeight 
+    steelKind 
+    steelGrade 
+    slabLength 
+    slabNum 
+    slabThickness 
+    slabWidth 
+  }
+}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT coil_no as coilNum, coil_status as coilStatus, coil_weight as coilWeight, steel_kind as steelKind, steel_grade as steelGrade,
+slab_length as slabLength, slab_num as slabNum, slab_thickness as slabThickness, slab_width as slabWidth FROM public.steel_coil where coil_status = true;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Successfully</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ansteel-function-test-9</t>
+  </si>
+  <si>
+    <t>获取在生产的钢卷condition(_eq)
+order(`coilNum` ASC)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+  Coil(cond:"{coilStatus:{_eq:\"true\"}}", authInfo:"", order:"coilNum ASC")
+  {
+    coilNum 
+    coilStatus 
+    coilWeight 
+    steelKind 
+    steelGrade 
+    slabLength 
+    slabNum 
+    slabThickness 
+    slabWidth 
+  }
+}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT coil_no as coilNum, coil_status as coilStatus, coil_weight as coilWeight, steel_kind as steelKind, steel_grade as steelGrade,
+slab_length as slabLength, slab_num as slabNum, slab_thickness as slabThickness, slab_width as slabWidth FROM public.steel_coil where coil_status = true order by coil_no ASC;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ansteel-function-test-10</t>
+  </si>
+  <si>
+    <t>获取在生产的钢卷condition(_eq)
+order(`coilNum` ASC)pageIndex:1
+pageSize:20</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CoilConnection-&gt;edges</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+  CoilConnection(cond:"", authInfo:"", order:"", after:"1", first:20)
+  {
+    totalElements
+    totalPages
+    pageSize
+    page
+    numberOfElements
+    edges {
+      node {
+        slabNum
+        coilNum
+        id
+        coilWeight
+        slabWidth
+        coilStatus
+        slabLength
+        slabThickness
+        steelKind
+        steelGrade
+      }
+    }
+  }
+}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT coil_no as coilNum, coil_status as coilStatus, coil_weight as coilWeight, steel_kind as steelKind, steel_grade as steelGrade,
+slab_length as slabLength, slab_num as slabNum, slab_thickness as slabThickness, slab_width as slabWidth FROM public.steel_coil where coil_status = true order by coil_no ASC limit 20;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ansteel-function-test-11</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取钢卷Event</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Event</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">			{
+			  Event(cond:"{coilNum:{_in:[\"P011N00700\",\"P011C10400\",\"P011N00300\",\"P011C05000\"]}}", authInfo:"", order:"")
+			  {
+				timestamp
+				eventTag
+				processNum
+				device
+				coilNum
+			  }
+			}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>chdb</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT `timestamp`,eventTag,processNum,device,coilNum from Event_local el WHERE coilNum IN ('P011N00700','P011C10400','P011N00300','P011C05000');</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -664,13 +810,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13585E94-2A3C-423F-8526-0CA62361FED2}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.44140625" style="1" bestFit="1" customWidth="1"/>
@@ -684,7 +830,7 @@
     <col min="10" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -713,7 +859,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="150" customHeight="1">
+    <row r="2" spans="1:9" ht="150" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>15</v>
       </c>
@@ -742,7 +888,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="150" customHeight="1">
+    <row r="3" spans="1:9" ht="150" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>16</v>
       </c>
@@ -771,7 +917,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="150" customHeight="1">
+    <row r="4" spans="1:9" ht="150" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>17</v>
       </c>
@@ -800,7 +946,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="150" customHeight="1">
+    <row r="5" spans="1:9" ht="150" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
@@ -829,7 +975,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="150" customHeight="1">
+    <row r="6" spans="1:9" ht="150" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>20</v>
       </c>
@@ -858,7 +1004,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="150" customHeight="1">
+    <row r="7" spans="1:9" ht="150" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>39</v>
       </c>
@@ -878,7 +1024,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="150" customHeight="1">
+    <row r="8" spans="1:9" ht="150" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>40</v>
       </c>
@@ -905,6 +1051,122 @@
       </c>
       <c r="I8" s="5" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="184.8" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" s="1">
+        <v>200</v>
+      </c>
+      <c r="H9" s="1">
+        <v>100000</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="198" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G10" s="1">
+        <v>200</v>
+      </c>
+      <c r="H10" s="1">
+        <v>100000</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="316.8" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G11" s="1">
+        <v>200</v>
+      </c>
+      <c r="H11" s="1">
+        <v>100000</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" customFormat="1" ht="158.4" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G12" s="1">
+        <v>200</v>
+      </c>
+      <c r="H12" s="1">
+        <v>100000</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add new case of sdl-8818
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/ansteel-api-engine-test-data.xlsx
+++ b/src/main/resources/test-data-xls/ansteel-api-engine-test-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\auto_worksapce\feature-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8C4CDAC-9434-494B-B710-82759642D399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08C63AFA-B4E5-4824-90A4-BE1FA94FD0E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="80">
   <si>
     <t>description</t>
   </si>
@@ -165,6 +165,217 @@
 }</t>
   </si>
   <si>
+    <t>Alarm_DataConnection-&gt;edges</t>
+  </si>
+  <si>
+    <t>获取过程参数数据</t>
+  </si>
+  <si>
+    <t>database</t>
+  </si>
+  <si>
+    <t>chdb</t>
+  </si>
+  <si>
+    <t>SELECT cmdPoint ,`timestamp` ,alarmRuleId,alarmType,sensorId,absValue,processNum,coilNum FROM  chdb.Alarm_Data ad 
+WHERE `timestamp` &gt;= '2022-01-03 07:00:00.000' and `timestamp` &lt;= '2022-01-03 08:00:00.000' order by `timestamp` DESC;</t>
+  </si>
+  <si>
+    <t>SELECT cmdPoint ,`timestamp` ,alarmRuleId,alarmType,sensorId,absValue,processNum,coilNum FROM  chdb.Alarm_Data ad 
+WHERE `timestamp` &gt;= '2022-01-03 07:00:00.000' and `timestamp` &lt;= '2022-01-03 08:00:00.000' order by `timestamp` ASC limit 20;</t>
+  </si>
+  <si>
+    <t>SELECT cmdPoint ,`timestamp` ,alarmRuleId,alarmType,sensorId,absValue,processNum,coilNum FROM  chdb.Alarm_Data ad 
+WHERE processNum = 'FCE' order by `timestamp` ASC limit 20;</t>
+  </si>
+  <si>
+    <t>datacleaning</t>
+  </si>
+  <si>
+    <t>datamanagement</t>
+  </si>
+  <si>
+    <t>获取全产线报警最频繁的过程参数
+condition(_gte,_lte)
+order(`createTime` ASC)</t>
+  </si>
+  <si>
+    <t>{
+  Alarm_TopN(cond:"{createTime:{_gte:\"2022-05-17 00:00:00.000\",_lte:\"2022-05-17 23:59:59.000\"}}", authInfo:"", order:"createTime ASC")
+  {
+    count
+    coilNum
+    sensorId
+    createTime
+    id
+    period
+    periodEndTime
+    periodStartTime
+  }
+}</t>
+  </si>
+  <si>
+    <t>select * from public.datalayer_alarm_topn where create_time &gt;= '2022-05-17 00:00:00.000' 
+and create_time &lt;= '2022-05-17 23:59:59.000' order by create_time asc</t>
+  </si>
+  <si>
+    <t>ansteel-function-test-6</t>
+  </si>
+  <si>
+    <t>ansteel-function-test-7</t>
+  </si>
+  <si>
+    <t>Sensor</t>
+  </si>
+  <si>
+    <t>Alarm_TopN</t>
+  </si>
+  <si>
+    <t>ansteel-function-test-8</t>
+  </si>
+  <si>
+    <t>Coil</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+  Coil(cond:"{coilStatus:{_eq:\"true\"}}", authInfo:"", order:"")
+  {
+    coilNum 
+    coilStatus 
+    coilWeight 
+    steelKind 
+    steelGrade 
+    slabLength 
+    slabNum 
+    slabThickness 
+    slabWidth 
+  }
+}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT coil_no as coilNum, coil_status as coilStatus, coil_weight as coilWeight, steel_kind as steelKind, steel_grade as steelGrade,
+slab_length as slabLength, slab_num as slabNum, slab_thickness as slabThickness, slab_width as slabWidth FROM public.steel_coil where coil_status = true;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Successfully</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ansteel-function-test-9</t>
+  </si>
+  <si>
+    <t>获取在生产的钢卷condition(_eq)
+order(`coilNum` ASC)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+  Coil(cond:"{coilStatus:{_eq:\"true\"}}", authInfo:"", order:"coilNum ASC")
+  {
+    coilNum 
+    coilStatus 
+    coilWeight 
+    steelKind 
+    steelGrade 
+    slabLength 
+    slabNum 
+    slabThickness 
+    slabWidth 
+  }
+}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT coil_no as coilNum, coil_status as coilStatus, coil_weight as coilWeight, steel_kind as steelKind, steel_grade as steelGrade,
+slab_length as slabLength, slab_num as slabNum, slab_thickness as slabThickness, slab_width as slabWidth FROM public.steel_coil where coil_status = true order by coil_no ASC;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ansteel-function-test-10</t>
+  </si>
+  <si>
+    <t>CoilConnection-&gt;edges</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+  CoilConnection(cond:"", authInfo:"", order:"", after:"1", first:20)
+  {
+    totalElements
+    totalPages
+    pageSize
+    page
+    numberOfElements
+    edges {
+      node {
+        slabNum
+        coilNum
+        id
+        coilWeight
+        slabWidth
+        coilStatus
+        slabLength
+        slabThickness
+        steelKind
+        steelGrade
+      }
+    }
+  }
+}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT coil_no as coilNum, coil_status as coilStatus, coil_weight as coilWeight, steel_kind as steelKind, steel_grade as steelGrade,
+slab_length as slabLength, slab_num as slabNum, slab_thickness as slabThickness, slab_width as slabWidth FROM public.steel_coil where coil_status = true order by coil_no ASC limit 20;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ansteel-function-test-11</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Event</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>chdb</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>chdb</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Successfully</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ansteel-function-test-13</t>
+  </si>
+  <si>
+    <t>ansteel-function-test-14</t>
+  </si>
+  <si>
+    <t>获取钢卷Event condition(_like)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>按时间获取Event condition(_and)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取钢卷Event condition(_in)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT cmdPoint ,`timestamp` ,alarmRuleId,alarmType,sensorId,absValue,processNum,coilNum FROM chdb.Alarm_Data ad 
+WHERE `timestamp` &gt;= '2022-01-03 07:00:00.000' and `timestamp` &lt;= '2022-01-03 08:00:00.000' order by `timestamp` ASC;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>{
   Alarm_DataConnection(cond:"{timestamp:{_gte:\"2022-01-03 07:00:00.000\",_lte:\"2022-01-03 08:00:00.000\"}}", authInfo:"", order:"timestamp ASC", after:"1", first:20)
   {
@@ -188,9 +399,7 @@
     }
   }
 }</t>
-  </si>
-  <si>
-    <t>Alarm_DataConnection-&gt;edges</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>{
@@ -218,208 +427,18 @@
     type
   }
 }</t>
-  </si>
-  <si>
-    <t>获取过程参数数据</t>
-  </si>
-  <si>
-    <t>database</t>
-  </si>
-  <si>
-    <t>chdb</t>
-  </si>
-  <si>
-    <t>SELECT cmdPoint ,`timestamp` ,alarmRuleId,alarmType,sensorId,absValue,processNum,coilNum FROM chdb.Alarm_Data ad 
-WHERE `timestamp` &gt;= '2022-01-03 07:00:00.000' and `timestamp` &lt;= '2022-01-03 08:00:00.000' order by `timestamp` ASC;</t>
-  </si>
-  <si>
-    <t>SELECT cmdPoint ,`timestamp` ,alarmRuleId,alarmType,sensorId,absValue,processNum,coilNum FROM  chdb.Alarm_Data ad 
-WHERE `timestamp` &gt;= '2022-01-03 07:00:00.000' and `timestamp` &lt;= '2022-01-03 08:00:00.000' order by `timestamp` DESC;</t>
-  </si>
-  <si>
-    <t>SELECT cmdPoint ,`timestamp` ,alarmRuleId,alarmType,sensorId,absValue,processNum,coilNum FROM  chdb.Alarm_Data ad 
-WHERE `timestamp` &gt;= '2022-01-03 07:00:00.000' and `timestamp` &lt;= '2022-01-03 08:00:00.000' order by `timestamp` ASC limit 20;</t>
-  </si>
-  <si>
-    <t>SELECT cmdPoint ,`timestamp` ,alarmRuleId,alarmType,sensorId,absValue,processNum,coilNum FROM  chdb.Alarm_Data ad 
-WHERE processNum = 'FCE' order by `timestamp` ASC limit 20;</t>
-  </si>
-  <si>
-    <t>datacleaning</t>
-  </si>
-  <si>
-    <t>datamanagement</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>select pass,source,unit,rate,process as processNum,coil_id_no as coilIdNo,coil_id_no as coilIdNo,internal_sensor_name as internalSensorName,
 freq as frequency,pda_abs_addr as frequency,pda_abs_addr as pdaAddress,multiple_setting as physicalMeaning,process_range as processRange,
 source_sensor_name as sourceSensorName,description as sensorDescription,event_status as eventStatus,event_tag as eventTag,
 if_id as ifId,l2_l1_diff as diffL2L1,internal_sensor_name as id,device,type from public.sensor s where process = 'FCE';</t>
-  </si>
-  <si>
-    <t>获取全产线报警最频繁的过程参数
-condition(_gte,_lte)
-order(`createTime` ASC)</t>
-  </si>
-  <si>
-    <t>{
-  Alarm_TopN(cond:"{createTime:{_gte:\"2022-05-17 00:00:00.000\",_lte:\"2022-05-17 23:59:59.000\"}}", authInfo:"", order:"createTime ASC")
-  {
-    count
-    coilNum
-    sensorId
-    createTime
-    id
-    period
-    periodEndTime
-    periodStartTime
-  }
-}</t>
-  </si>
-  <si>
-    <t>select * from public.datalayer_alarm_topn where create_time &gt;= '2022-05-17 00:00:00.000' 
-and create_time &lt;= '2022-05-17 23:59:59.000' order by create_time asc</t>
-  </si>
-  <si>
-    <t>ansteel-function-test-6</t>
-  </si>
-  <si>
-    <t>ansteel-function-test-7</t>
-  </si>
-  <si>
-    <t>Sensor</t>
-  </si>
-  <si>
-    <t>Alarm_TopN</t>
-  </si>
-  <si>
-    <t>ansteel-function-test-8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">获取在生产的钢卷condition(_eq)
-order(`timestamp` ASC)	</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Coil</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>{
-  Coil(cond:"{coilStatus:{_eq:\"true\"}}", authInfo:"", order:"")
-  {
-    coilNum 
-    coilStatus 
-    coilWeight 
-    steelKind 
-    steelGrade 
-    slabLength 
-    slabNum 
-    slabThickness 
-    slabWidth 
-  }
-}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SELECT coil_no as coilNum, coil_status as coilStatus, coil_weight as coilWeight, steel_kind as steelKind, steel_grade as steelGrade,
-slab_length as slabLength, slab_num as slabNum, slab_thickness as slabThickness, slab_width as slabWidth FROM public.steel_coil where coil_status = true;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Successfully</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ansteel-function-test-9</t>
-  </si>
-  <si>
-    <t>获取在生产的钢卷condition(_eq)
-order(`coilNum` ASC)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>{
-  Coil(cond:"{coilStatus:{_eq:\"true\"}}", authInfo:"", order:"coilNum ASC")
-  {
-    coilNum 
-    coilStatus 
-    coilWeight 
-    steelKind 
-    steelGrade 
-    slabLength 
-    slabNum 
-    slabThickness 
-    slabWidth 
-  }
-}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SELECT coil_no as coilNum, coil_status as coilStatus, coil_weight as coilWeight, steel_kind as steelKind, steel_grade as steelGrade,
-slab_length as slabLength, slab_num as slabNum, slab_thickness as slabThickness, slab_width as slabWidth FROM public.steel_coil where coil_status = true order by coil_no ASC;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ansteel-function-test-10</t>
-  </si>
-  <si>
-    <t>获取在生产的钢卷condition(_eq)
-order(`coilNum` ASC)pageIndex:1
-pageSize:20</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CoilConnection-&gt;edges</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>{
-  CoilConnection(cond:"", authInfo:"", order:"", after:"1", first:20)
-  {
-    totalElements
-    totalPages
-    pageSize
-    page
-    numberOfElements
-    edges {
-      node {
-        slabNum
-        coilNum
-        id
-        coilWeight
-        slabWidth
-        coilStatus
-        slabLength
-        slabThickness
-        steelKind
-        steelGrade
-      }
-    }
-  }
-}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SELECT coil_no as coilNum, coil_status as coilStatus, coil_weight as coilWeight, steel_kind as steelKind, steel_grade as steelGrade,
-slab_length as slabLength, slab_num as slabNum, slab_thickness as slabThickness, slab_width as slabWidth FROM public.steel_coil where coil_status = true order by coil_no ASC limit 20;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ansteel-function-test-11</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>获取钢卷Event</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Event</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">			{
-			  Event(cond:"{coilNum:{_in:[\"P011N00700\",\"P011C10400\",\"P011N00300\",\"P011C05000\"]}}", authInfo:"", order:"")
+			  Event(cond:"{coilNum:{_in:[\"P011N00700\",\"P011C10400\",\"P011N00300\",\"P011C05000\"]}}", authInfo:"", order:"timestamp ASC")
 			  {
 				timestamp
 				eventTag
@@ -431,11 +450,84 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>SELECT `timestamp`,eventTag,processNum,device,coilNum from Event_local el WHERE coilNum IN ('P011N00700','P011C10400','P011N00300','P011C05000') order by `timestamp` ASC;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+			  Event(cond:"{_and:[{timestamp:{_lt:\"2022-01-02 08:30:00.000\"}},{timestamp:{_gte:\"2022-01-02 08:20:00.000\"}}]}", authInfo:"", order:"timestamp ASC")
+			  {
+		                        timestamp
+				eventTag
+				processNum
+                                                device
+				coilNum
+			  }
+			}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">获取在生产的钢卷condition(_eq)	</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取在生产的钢卷condition(_eq)pageIndex:1
+pageSize:20</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ansteel-function-test-15</t>
+  </si>
+  <si>
+    <t>SELECT `timestamp`,eventTag,processNum,device,coilNum from Event_local el 
+where `timestamp` &gt;= '2022-01-02 08:20:00.000' and `timestamp` &lt; '2022-01-02 08:30:00.000' order by `timestamp` ASC;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Successfully</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>按时间获取Event condition(_or)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>chdb</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>SELECT `timestamp`,eventTag,processNum,device,coilNum from Event_local el WHERE coilNum IN ('P011N00700','P011C10400','P011N00300','P011C05000');</t>
+    <t>SELECT `timestamp`,eventTag,processNum,device,coilNum from Event_local el WHERE coilNum LIKE '%P010N00%' order by `timestamp` ASC;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">	 {
+			  Event(cond:"{coilNum:{_like: \"%P010N00%\"}}", order:"timestamp ASC")
+			  {
+				timestamp
+				eventTag
+				processNum
+                                                device
+				coilNum
+			  }
+			}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+			  Event(cond:"{_or:[{timestamp:{_lt:\"2022-01-02 08:00:00.000\"}},{timestamp:{_gte:\"2022-01-03 07:30:00.000\"}}]}", authInfo:"", order:"timestamp ASC")
+			  {
+		                        timestamp
+				eventTag
+				processNum
+                                                device
+				coilNum
+			  }
+			}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT `timestamp`,eventTag,processNum,device,coilNum from Event_local el 
+where `timestamp` &lt; '2022-01-02 08:00:00.000' or `timestamp` &gt;= '2022-01-03 07:30:00.000' order by `timestamp` ASC;</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -810,10 +902,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13585E94-2A3C-423F-8526-0CA62361FED2}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -825,7 +917,7 @@
     <col min="5" max="5" width="14.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="56.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="8.88671875" style="1"/>
   </cols>
@@ -844,7 +936,7 @@
         <v>5</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>7</v>
@@ -873,10 +965,10 @@
         <v>21</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>29</v>
+        <v>62</v>
       </c>
       <c r="G2" s="5">
         <v>200</v>
@@ -902,10 +994,10 @@
         <v>22</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G3" s="5">
         <v>200</v>
@@ -925,16 +1017,16 @@
         <v>12</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>23</v>
+        <v>63</v>
       </c>
       <c r="E4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>31</v>
       </c>
       <c r="G4" s="5">
         <v>200</v>
@@ -954,16 +1046,16 @@
         <v>13</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G5" s="5">
         <v>200</v>
@@ -983,16 +1075,16 @@
         <v>19</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>25</v>
+        <v>64</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>35</v>
+        <v>65</v>
       </c>
       <c r="G6" s="5">
         <v>200</v>
@@ -1006,10 +1098,10 @@
     </row>
     <row r="7" spans="1:9" ht="150" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="3"/>
@@ -1026,22 +1118,22 @@
     </row>
     <row r="8" spans="1:9" ht="150" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>38</v>
       </c>
       <c r="G8" s="5">
         <v>200</v>
@@ -1055,22 +1147,22 @@
     </row>
     <row r="9" spans="1:9" ht="184.8" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>44</v>
+        <v>69</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="G9" s="1">
         <v>200</v>
@@ -1079,27 +1171,27 @@
         <v>100000</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="198" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="G10" s="1">
         <v>200</v>
@@ -1108,27 +1200,27 @@
         <v>100000</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="316.8" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="G11" s="1">
         <v>200</v>
@@ -1137,27 +1229,27 @@
         <v>100000</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:9" customFormat="1" ht="158.4" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="G12" s="1">
         <v>200</v>
@@ -1166,7 +1258,94 @@
         <v>100000</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="132" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G13" s="1">
+        <v>200</v>
+      </c>
+      <c r="H13" s="1">
+        <v>100000</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="158.4" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G14" s="1">
+        <v>200</v>
+      </c>
+      <c r="H14" s="1">
+        <v>100000</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="158.4" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G15" s="1">
+        <v>200</v>
+      </c>
+      <c r="H15" s="1">
+        <v>100000</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add new case of ansteel dev
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/ansteel-api-engine-test-data.xlsx
+++ b/src/main/resources/test-data-xls/ansteel-api-engine-test-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\auto_worksapce\feature-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08C63AFA-B4E5-4824-90A4-BE1FA94FD0E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7039E8DB-A41B-48BF-90C3-2C1C83484153}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="86">
   <si>
     <t>description</t>
   </si>
@@ -78,13 +78,6 @@
   <si>
     <t>获取过程参数预警列表
 condition(_gte,_lte)
-order(`timestamp` ASC)
-pageIndex:1
-pageSize:20</t>
-  </si>
-  <si>
-    <t>获取过程参数预警列表
-condition(_eq)
 order(`timestamp` ASC)
 pageIndex:1
 pageSize:20</t>
@@ -267,11 +260,6 @@
     <t>ansteel-function-test-9</t>
   </si>
   <si>
-    <t>获取在生产的钢卷condition(_eq)
-order(`coilNum` ASC)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>{
   Coil(cond:"{coilStatus:{_eq:\"true\"}}", authInfo:"", order:"coilNum ASC")
   {
@@ -301,33 +289,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>{
-  CoilConnection(cond:"", authInfo:"", order:"", after:"1", first:20)
-  {
-    totalElements
-    totalPages
-    pageSize
-    page
-    numberOfElements
-    edges {
-      node {
-        slabNum
-        coilNum
-        id
-        coilWeight
-        slabWidth
-        coilStatus
-        slabLength
-        slabThickness
-        steelKind
-        steelGrade
-      }
-    }
-  }
-}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>SELECT coil_no as coilNum, coil_status as coilStatus, coil_weight as coilWeight, steel_kind as steelKind, steel_grade as steelGrade,
 slab_length as slabLength, slab_num as slabNum, slab_thickness as slabThickness, slab_width as slabWidth FROM public.steel_coil where coil_status = true order by coil_no ASC limit 20;</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -357,18 +318,6 @@
   </si>
   <si>
     <t>ansteel-function-test-14</t>
-  </si>
-  <si>
-    <t>获取钢卷Event condition(_like)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>按时间获取Event condition(_and)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>获取钢卷Event condition(_in)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>SELECT cmdPoint ,`timestamp` ,alarmRuleId,alarmType,sensorId,absValue,processNum,coilNum FROM chdb.Alarm_Data ad 
@@ -454,34 +403,7 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>{
-			  Event(cond:"{_and:[{timestamp:{_lt:\"2022-01-02 08:30:00.000\"}},{timestamp:{_gte:\"2022-01-02 08:20:00.000\"}}]}", authInfo:"", order:"timestamp ASC")
-			  {
-		                        timestamp
-				eventTag
-				processNum
-                                                device
-				coilNum
-			  }
-			}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">获取在生产的钢卷condition(_eq)	</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>获取在生产的钢卷condition(_eq)pageIndex:1
-pageSize:20</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>ansteel-function-test-15</t>
-  </si>
-  <si>
-    <t>SELECT `timestamp`,eventTag,processNum,device,coilNum from Event_local el 
-where `timestamp` &gt;= '2022-01-02 08:20:00.000' and `timestamp` &lt; '2022-01-02 08:30:00.000' order by `timestamp` ASC;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Successfully</t>
@@ -513,8 +435,97 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>ansteel-function-test-16</t>
+  </si>
+  <si>
+    <t>Successfully</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">生成节奏监控 获取在生产的钢卷condition(_eq)	</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>生成节奏监控 获取在生产的钢卷condition(_eq)
+order(`coilNum` ASC)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>生成节奏监控 获取在生产的钢卷condition(_eq)pageIndex:1
+pageSize:20</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>生成节奏监控 获取钢卷Event condition(_in)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>生成节奏监控 获取钢卷Event condition(_like)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>生成节奏监控 按时间获取Event condition(_and)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取过程参数预警列表
+condition(_eq)
+order(`timestamp` ASC)
+pageIndex:1
+pageSize:20</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>{
-			  Event(cond:"{_or:[{timestamp:{_lt:\"2022-01-02 08:00:00.000\"}},{timestamp:{_gte:\"2022-01-03 07:30:00.000\"}}]}", authInfo:"", order:"timestamp ASC")
+  CoilConnection(cond:"{coilStatus:{_eq:\"true\"}}", authInfo:"", order:"coilStatus ASC", after:"1", first:20)
+  {
+    totalElements
+    totalPages
+    pageSize
+    page
+    numberOfElements
+    edges {
+      node {
+        slabNum
+        coilNum
+        id
+        coilWeight
+        slabWidth
+        coilStatus
+        slabLength
+        slabThickness
+        steelKind
+        steelGrade
+      }
+    }
+  }
+}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>nestedEntityWithCondition</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>温度仿真 获取正在生产的钢卷对象 condition(_eq and)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  {Coil(cond:"{coilStatus:{_eq:false}}",authInfo:"",order:"") {steelKind steelGrade slabWidth coilStatus slabThickness coilWeight slabLength slabNum coilNum id link_Event(cond:"{_and:[{processNum:{_eq:\"FCE\"}},{eventTag:{_eq:\"in\"}}]}",authInfo:"",order:"") { timestamp device eventTag processNum coilNum }}}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>link_Event,processNum,FCE,eventTag,in</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT `timestamp`,eventTag,processNum,device,coilNum from Event_local el 
+where `timestamp` &gt;= '2022-01-02 08:20:56.000' and `timestamp` &lt; '2022-01-02 08:21:00.000' order by `timestamp` ASC;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+			  Event(cond:"{_and:[{timestamp:{_lt:\"2022-01-02 08:21:00.000\"}},{timestamp:{_gte:\"2022-01-02 08:20:56.000\"}}]}", authInfo:"", order:"timestamp ASC")
 			  {
 		                        timestamp
 				eventTag
@@ -527,7 +538,20 @@
   </si>
   <si>
     <t>SELECT `timestamp`,eventTag,processNum,device,coilNum from Event_local el 
-where `timestamp` &lt; '2022-01-02 08:00:00.000' or `timestamp` &gt;= '2022-01-03 07:30:00.000' order by `timestamp` ASC;</t>
+where `timestamp` &lt; '2022-01-02 08:00:00.000' or `timestamp` &gt;= '2022-01-03 08:05:34.000' order by `timestamp` ASC;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+			  Event(cond:"{_or:[{timestamp:{_lt:\"2022-01-02 08:00:00.000\"}},{timestamp:{_gte:\"2022-01-03 08:05:34.000\"}}]}", authInfo:"", order:"timestamp ASC")
+			  {
+		                        timestamp
+				eventTag
+				processNum
+                                                device
+				coilNum
+			  }
+			}</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -902,10 +926,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13585E94-2A3C-423F-8526-0CA62361FED2}">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -913,16 +937,17 @@
     <col min="1" max="1" width="12.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="59.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="71" style="1" customWidth="1"/>
     <col min="5" max="5" width="14.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="56.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="1"/>
+    <col min="7" max="7" width="56.44140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -936,24 +961,27 @@
         <v>5</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="150" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="150" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>10</v>
@@ -962,27 +990,28 @@
         <v>9</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="G2" s="5">
+        <v>56</v>
+      </c>
+      <c r="G2" s="3"/>
+      <c r="H2" s="5">
         <v>200</v>
       </c>
-      <c r="H2" s="5">
+      <c r="I2" s="5">
         <v>100000</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="150" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="150" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>11</v>
@@ -991,361 +1020,393 @@
         <v>9</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" s="5">
+      <c r="G3" s="3"/>
+      <c r="H3" s="5">
         <v>200</v>
       </c>
-      <c r="H3" s="5">
+      <c r="I3" s="5">
         <v>100000</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="J3" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="150" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="150" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="3"/>
+      <c r="H4" s="5">
+        <v>200</v>
+      </c>
+      <c r="I4" s="5">
+        <v>100000</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="150" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="3"/>
+      <c r="H5" s="5">
+        <v>200</v>
+      </c>
+      <c r="I5" s="5">
+        <v>100000</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="150" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G6" s="3"/>
+      <c r="H6" s="5">
+        <v>200</v>
+      </c>
+      <c r="I6" s="5">
+        <v>100000</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="150" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" s="5">
-        <v>200</v>
-      </c>
-      <c r="H4" s="5">
-        <v>100000</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="150" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G5" s="5">
-        <v>200</v>
-      </c>
-      <c r="H5" s="5">
-        <v>100000</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="150" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="G6" s="5">
-        <v>200</v>
-      </c>
-      <c r="H6" s="5">
-        <v>100000</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="150" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>24</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
-      <c r="G7" s="5">
+      <c r="H7" s="5">
         <v>200</v>
       </c>
-      <c r="H7" s="5">
+      <c r="I7" s="5">
         <v>100000</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="J7" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="150" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="150" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="E8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="3"/>
+      <c r="H8" s="5">
+        <v>200</v>
+      </c>
+      <c r="I8" s="5">
+        <v>100000</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="184.8" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="G8" s="5">
+      <c r="B9" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H9" s="1">
         <v>200</v>
       </c>
-      <c r="H8" s="5">
+      <c r="I9" s="1">
         <v>100000</v>
       </c>
-      <c r="I8" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="184.8" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="J9" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="184.8" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="D10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H10" s="1">
+        <v>200</v>
+      </c>
+      <c r="I10" s="1">
+        <v>100000</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="330" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H11" s="1">
+        <v>200</v>
+      </c>
+      <c r="I11" s="1">
+        <v>100000</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" customFormat="1" ht="158.4" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1">
+        <v>200</v>
+      </c>
+      <c r="I12" s="1">
+        <v>100000</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="132" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H13" s="1">
+        <v>200</v>
+      </c>
+      <c r="I13" s="1">
+        <v>100000</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="158.4" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H14" s="1">
+        <v>200</v>
+      </c>
+      <c r="I14" s="1">
+        <v>100000</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="158.4" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H15" s="1">
+        <v>200</v>
+      </c>
+      <c r="I15" s="1">
+        <v>100000</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H16" s="1">
+        <v>200</v>
+      </c>
+      <c r="I16" s="1">
+        <v>100000</v>
+      </c>
+      <c r="J16" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G9" s="1">
-        <v>200</v>
-      </c>
-      <c r="H9" s="1">
-        <v>100000</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="198" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G10" s="1">
-        <v>200</v>
-      </c>
-      <c r="H10" s="1">
-        <v>100000</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="316.8" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G11" s="1">
-        <v>200</v>
-      </c>
-      <c r="H11" s="1">
-        <v>100000</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" customFormat="1" ht="158.4" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G12" s="1">
-        <v>200</v>
-      </c>
-      <c r="H12" s="1">
-        <v>100000</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="132" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="G13" s="1">
-        <v>200</v>
-      </c>
-      <c r="H13" s="1">
-        <v>100000</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="158.4" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="G14" s="1">
-        <v>200</v>
-      </c>
-      <c r="H14" s="1">
-        <v>100000</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="158.4" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="G15" s="1">
-        <v>200</v>
-      </c>
-      <c r="H15" s="1">
-        <v>100000</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add/update test cases for smart space
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/ansteel-api-engine-test-data.xlsx
+++ b/src/main/resources/test-data-xls/ansteel-api-engine-test-data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\auto_worksapce\feature-automation\src\main\resources\test-data-xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8C4CDAC-9434-494B-B710-82759642D399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A98E0835-EF5D-4735-BCCF-A2F0380FBCF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -443,31 +443,31 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -812,11 +812,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13585E94-2A3C-423F-8526-0CA62361FED2}">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="1" width="12.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.44140625" style="1" bestFit="1" customWidth="1"/>
@@ -830,7 +830,7 @@
     <col min="10" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -859,7 +859,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="150" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="150" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>15</v>
       </c>
@@ -888,7 +888,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="150" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="150" customHeight="1">
       <c r="A3" s="3" t="s">
         <v>16</v>
       </c>
@@ -917,7 +917,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="150" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="150" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>17</v>
       </c>
@@ -946,7 +946,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="150" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="150" customHeight="1">
       <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
@@ -975,7 +975,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="150" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="150" customHeight="1">
       <c r="A6" s="3" t="s">
         <v>20</v>
       </c>
@@ -1004,7 +1004,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="150" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="150" customHeight="1">
       <c r="A7" s="3" t="s">
         <v>39</v>
       </c>
@@ -1014,6 +1014,7 @@
       <c r="C7" s="4"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
       <c r="G7" s="5">
         <v>200</v>
       </c>
@@ -1024,7 +1025,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="150" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="150" customHeight="1">
       <c r="A8" s="3" t="s">
         <v>40</v>
       </c>
@@ -1053,119 +1054,119 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="184.8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="150" customHeight="1">
       <c r="A9" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G9" s="5">
         <v>200</v>
       </c>
-      <c r="H9" s="1">
+      <c r="H9" s="5">
         <v>100000</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="I9" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="198" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="150" customHeight="1">
       <c r="A10" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10" s="5">
         <v>200</v>
       </c>
-      <c r="H10" s="1">
+      <c r="H10" s="5">
         <v>100000</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="I10" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="316.8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="150" customHeight="1">
       <c r="A11" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G11" s="5">
         <v>200</v>
       </c>
-      <c r="H11" s="1">
+      <c r="H11" s="5">
         <v>100000</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="I11" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:9" customFormat="1" ht="158.4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="150" customHeight="1">
       <c r="A12" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="G12" s="1">
+      <c r="G12" s="5">
         <v>200</v>
       </c>
-      <c r="H12" s="1">
+      <c r="H12" s="5">
         <v>100000</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="I12" s="5" t="s">
         <v>48</v>
       </c>
     </row>

</xml_diff>

<commit_message>
revert to find back missing case
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/ansteel-api-engine-test-data.xlsx
+++ b/src/main/resources/test-data-xls/ansteel-api-engine-test-data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\data-layer-automation\src\main\resources\test-data-xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\auto_worksapce\feature-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A98E0835-EF5D-4735-BCCF-A2F0380FBCF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F956D241-BD26-48D2-97AF-AD0A80C096A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="93">
   <si>
     <t>description</t>
   </si>
@@ -78,13 +78,6 @@
   <si>
     <t>获取过程参数预警列表
 condition(_gte,_lte)
-order(`timestamp` ASC)
-pageIndex:1
-pageSize:20</t>
-  </si>
-  <si>
-    <t>获取过程参数预警列表
-condition(_eq)
 order(`timestamp` ASC)
 pageIndex:1
 pageSize:20</t>
@@ -165,6 +158,173 @@
 }</t>
   </si>
   <si>
+    <t>Alarm_DataConnection-&gt;edges</t>
+  </si>
+  <si>
+    <t>获取过程参数数据</t>
+  </si>
+  <si>
+    <t>database</t>
+  </si>
+  <si>
+    <t>chdb</t>
+  </si>
+  <si>
+    <t>SELECT cmdPoint ,`timestamp` ,alarmRuleId,alarmType,sensorId,absValue,processNum,coilNum FROM  chdb.Alarm_Data ad 
+WHERE `timestamp` &gt;= '2022-01-03 07:00:00.000' and `timestamp` &lt;= '2022-01-03 08:00:00.000' order by `timestamp` DESC;</t>
+  </si>
+  <si>
+    <t>SELECT cmdPoint ,`timestamp` ,alarmRuleId,alarmType,sensorId,absValue,processNum,coilNum FROM  chdb.Alarm_Data ad 
+WHERE `timestamp` &gt;= '2022-01-03 07:00:00.000' and `timestamp` &lt;= '2022-01-03 08:00:00.000' order by `timestamp` ASC limit 20;</t>
+  </si>
+  <si>
+    <t>SELECT cmdPoint ,`timestamp` ,alarmRuleId,alarmType,sensorId,absValue,processNum,coilNum FROM  chdb.Alarm_Data ad 
+WHERE processNum = 'FCE' order by `timestamp` ASC limit 20;</t>
+  </si>
+  <si>
+    <t>datacleaning</t>
+  </si>
+  <si>
+    <t>datamanagement</t>
+  </si>
+  <si>
+    <t>获取全产线报警最频繁的过程参数
+condition(_gte,_lte)
+order(`createTime` ASC)</t>
+  </si>
+  <si>
+    <t>{
+  Alarm_TopN(cond:"{createTime:{_gte:\"2022-05-17 00:00:00.000\",_lte:\"2022-05-17 23:59:59.000\"}}", authInfo:"", order:"createTime ASC")
+  {
+    count
+    coilNum
+    sensorId
+    createTime
+    id
+    period
+    periodEndTime
+    periodStartTime
+  }
+}</t>
+  </si>
+  <si>
+    <t>select * from public.datalayer_alarm_topn where create_time &gt;= '2022-05-17 00:00:00.000' 
+and create_time &lt;= '2022-05-17 23:59:59.000' order by create_time asc</t>
+  </si>
+  <si>
+    <t>ansteel-function-test-6</t>
+  </si>
+  <si>
+    <t>ansteel-function-test-7</t>
+  </si>
+  <si>
+    <t>Sensor</t>
+  </si>
+  <si>
+    <t>Alarm_TopN</t>
+  </si>
+  <si>
+    <t>ansteel-function-test-8</t>
+  </si>
+  <si>
+    <t>Coil</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+  Coil(cond:"{coilStatus:{_eq:\"true\"}}", authInfo:"", order:"")
+  {
+    coilNum 
+    coilStatus 
+    coilWeight 
+    steelKind 
+    steelGrade 
+    slabLength 
+    slabNum 
+    slabThickness 
+    slabWidth 
+  }
+}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT coil_no as coilNum, coil_status as coilStatus, coil_weight as coilWeight, steel_kind as steelKind, steel_grade as steelGrade,
+slab_length as slabLength, slab_num as slabNum, slab_thickness as slabThickness, slab_width as slabWidth FROM public.steel_coil where coil_status = true;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Successfully</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ansteel-function-test-9</t>
+  </si>
+  <si>
+    <t>{
+  Coil(cond:"{coilStatus:{_eq:\"true\"}}", authInfo:"", order:"coilNum ASC")
+  {
+    coilNum 
+    coilStatus 
+    coilWeight 
+    steelKind 
+    steelGrade 
+    slabLength 
+    slabNum 
+    slabThickness 
+    slabWidth 
+  }
+}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT coil_no as coilNum, coil_status as coilStatus, coil_weight as coilWeight, steel_kind as steelKind, steel_grade as steelGrade,
+slab_length as slabLength, slab_num as slabNum, slab_thickness as slabThickness, slab_width as slabWidth FROM public.steel_coil where coil_status = true order by coil_no ASC;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ansteel-function-test-10</t>
+  </si>
+  <si>
+    <t>CoilConnection-&gt;edges</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT coil_no as coilNum, coil_status as coilStatus, coil_weight as coilWeight, steel_kind as steelKind, steel_grade as steelGrade,
+slab_length as slabLength, slab_num as slabNum, slab_thickness as slabThickness, slab_width as slabWidth FROM public.steel_coil where coil_status = true order by coil_no ASC limit 20;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ansteel-function-test-11</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Event</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>chdb</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>chdb</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Successfully</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ansteel-function-test-13</t>
+  </si>
+  <si>
+    <t>ansteel-function-test-14</t>
+  </si>
+  <si>
+    <t>SELECT cmdPoint ,`timestamp` ,alarmRuleId,alarmType,sensorId,absValue,processNum,coilNum FROM chdb.Alarm_Data ad 
+WHERE `timestamp` &gt;= '2022-01-03 07:00:00.000' and `timestamp` &lt;= '2022-01-03 08:00:00.000' order by `timestamp` ASC;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>{
   Alarm_DataConnection(cond:"{timestamp:{_gte:\"2022-01-03 07:00:00.000\",_lte:\"2022-01-03 08:00:00.000\"}}", authInfo:"", order:"timestamp ASC", after:"1", first:20)
   {
@@ -188,9 +348,7 @@
     }
   }
 }</t>
-  </si>
-  <si>
-    <t>Alarm_DataConnection-&gt;edges</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>{
@@ -218,164 +376,108 @@
     type
   }
 }</t>
-  </si>
-  <si>
-    <t>获取过程参数数据</t>
-  </si>
-  <si>
-    <t>database</t>
-  </si>
-  <si>
-    <t>chdb</t>
-  </si>
-  <si>
-    <t>SELECT cmdPoint ,`timestamp` ,alarmRuleId,alarmType,sensorId,absValue,processNum,coilNum FROM chdb.Alarm_Data ad 
-WHERE `timestamp` &gt;= '2022-01-03 07:00:00.000' and `timestamp` &lt;= '2022-01-03 08:00:00.000' order by `timestamp` ASC;</t>
-  </si>
-  <si>
-    <t>SELECT cmdPoint ,`timestamp` ,alarmRuleId,alarmType,sensorId,absValue,processNum,coilNum FROM  chdb.Alarm_Data ad 
-WHERE `timestamp` &gt;= '2022-01-03 07:00:00.000' and `timestamp` &lt;= '2022-01-03 08:00:00.000' order by `timestamp` DESC;</t>
-  </si>
-  <si>
-    <t>SELECT cmdPoint ,`timestamp` ,alarmRuleId,alarmType,sensorId,absValue,processNum,coilNum FROM  chdb.Alarm_Data ad 
-WHERE `timestamp` &gt;= '2022-01-03 07:00:00.000' and `timestamp` &lt;= '2022-01-03 08:00:00.000' order by `timestamp` ASC limit 20;</t>
-  </si>
-  <si>
-    <t>SELECT cmdPoint ,`timestamp` ,alarmRuleId,alarmType,sensorId,absValue,processNum,coilNum FROM  chdb.Alarm_Data ad 
-WHERE processNum = 'FCE' order by `timestamp` ASC limit 20;</t>
-  </si>
-  <si>
-    <t>datacleaning</t>
-  </si>
-  <si>
-    <t>datamanagement</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>select pass,source,unit,rate,process as processNum,coil_id_no as coilIdNo,coil_id_no as coilIdNo,internal_sensor_name as internalSensorName,
 freq as frequency,pda_abs_addr as frequency,pda_abs_addr as pdaAddress,multiple_setting as physicalMeaning,process_range as processRange,
 source_sensor_name as sourceSensorName,description as sensorDescription,event_status as eventStatus,event_tag as eventTag,
 if_id as ifId,l2_l1_diff as diffL2L1,internal_sensor_name as id,device,type from public.sensor s where process = 'FCE';</t>
-  </si>
-  <si>
-    <t>获取全产线报警最频繁的过程参数
-condition(_gte,_lte)
-order(`createTime` ASC)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">			{
+			  Event(cond:"{coilNum:{_in:[\"P011N00700\",\"P011C10400\",\"P011N00300\",\"P011C05000\"]}}", authInfo:"", order:"timestamp ASC")
+			  {
+				timestamp
+				eventTag
+				processNum
+				device
+				coilNum
+			  }
+			}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT `timestamp`,eventTag,processNum,device,coilNum from Event_local el WHERE coilNum IN ('P011N00700','P011C10400','P011N00300','P011C05000') order by `timestamp` ASC;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ansteel-function-test-15</t>
+  </si>
+  <si>
+    <t>Successfully</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>按时间获取Event condition(_or)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>chdb</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT `timestamp`,eventTag,processNum,device,coilNum from Event_local el WHERE coilNum LIKE '%P010N00%' order by `timestamp` ASC;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">	 {
+			  Event(cond:"{coilNum:{_like: \"%P010N00%\"}}", order:"timestamp ASC")
+			  {
+				timestamp
+				eventTag
+				processNum
+                                                device
+				coilNum
+			  }
+			}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ansteel-function-test-16</t>
+  </si>
+  <si>
+    <t>Successfully</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">生成节奏监控 获取在生产的钢卷condition(_eq)	</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>生成节奏监控 获取在生产的钢卷condition(_eq)
+order(`coilNum` ASC)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>生成节奏监控 获取在生产的钢卷condition(_eq)pageIndex:1
+pageSize:20</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>生成节奏监控 获取钢卷Event condition(_in)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>生成节奏监控 获取钢卷Event condition(_like)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>生成节奏监控 按时间获取Event condition(_and)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取过程参数预警列表
+condition(_eq)
+order(`timestamp` ASC)
+pageIndex:1
+pageSize:20</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>{
-  Alarm_TopN(cond:"{createTime:{_gte:\"2022-05-17 00:00:00.000\",_lte:\"2022-05-17 23:59:59.000\"}}", authInfo:"", order:"createTime ASC")
-  {
-    count
-    coilNum
-    sensorId
-    createTime
-    id
-    period
-    periodEndTime
-    periodStartTime
-  }
-}</t>
-  </si>
-  <si>
-    <t>select * from public.datalayer_alarm_topn where create_time &gt;= '2022-05-17 00:00:00.000' 
-and create_time &lt;= '2022-05-17 23:59:59.000' order by create_time asc</t>
-  </si>
-  <si>
-    <t>ansteel-function-test-6</t>
-  </si>
-  <si>
-    <t>ansteel-function-test-7</t>
-  </si>
-  <si>
-    <t>Sensor</t>
-  </si>
-  <si>
-    <t>Alarm_TopN</t>
-  </si>
-  <si>
-    <t>ansteel-function-test-8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">获取在生产的钢卷condition(_eq)
-order(`timestamp` ASC)	</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Coil</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>{
-  Coil(cond:"{coilStatus:{_eq:\"true\"}}", authInfo:"", order:"")
-  {
-    coilNum 
-    coilStatus 
-    coilWeight 
-    steelKind 
-    steelGrade 
-    slabLength 
-    slabNum 
-    slabThickness 
-    slabWidth 
-  }
-}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SELECT coil_no as coilNum, coil_status as coilStatus, coil_weight as coilWeight, steel_kind as steelKind, steel_grade as steelGrade,
-slab_length as slabLength, slab_num as slabNum, slab_thickness as slabThickness, slab_width as slabWidth FROM public.steel_coil where coil_status = true;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Successfully</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ansteel-function-test-9</t>
-  </si>
-  <si>
-    <t>获取在生产的钢卷condition(_eq)
-order(`coilNum` ASC)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>{
-  Coil(cond:"{coilStatus:{_eq:\"true\"}}", authInfo:"", order:"coilNum ASC")
-  {
-    coilNum 
-    coilStatus 
-    coilWeight 
-    steelKind 
-    steelGrade 
-    slabLength 
-    slabNum 
-    slabThickness 
-    slabWidth 
-  }
-}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SELECT coil_no as coilNum, coil_status as coilStatus, coil_weight as coilWeight, steel_kind as steelKind, steel_grade as steelGrade,
-slab_length as slabLength, slab_num as slabNum, slab_thickness as slabThickness, slab_width as slabWidth FROM public.steel_coil where coil_status = true order by coil_no ASC;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ansteel-function-test-10</t>
-  </si>
-  <si>
-    <t>获取在生产的钢卷condition(_eq)
-order(`coilNum` ASC)pageIndex:1
-pageSize:20</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CoilConnection-&gt;edges</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>{
-  CoilConnection(cond:"", authInfo:"", order:"", after:"1", first:20)
+  CoilConnection(cond:"{coilStatus:{_eq:\"true\"}}", authInfo:"", order:"coilStatus ASC", after:"1", first:20)
   {
     totalElements
     totalPages
@@ -401,41 +503,92 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>SELECT coil_no as coilNum, coil_status as coilStatus, coil_weight as coilWeight, steel_kind as steelKind, steel_grade as steelGrade,
-slab_length as slabLength, slab_num as slabNum, slab_thickness as slabThickness, slab_width as slabWidth FROM public.steel_coil where coil_status = true order by coil_no ASC limit 20;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ansteel-function-test-11</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>获取钢卷Event</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Event</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">			{
-			  Event(cond:"{coilNum:{_in:[\"P011N00700\",\"P011C10400\",\"P011N00300\",\"P011C05000\"]}}", authInfo:"", order:"")
+    <t>nestedEntityWithCondition</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>温度仿真 获取正在生产的钢卷对象 condition(_eq and)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  {Coil(cond:"{coilStatus:{_eq:false}}",authInfo:"",order:"") {steelKind steelGrade slabWidth coilStatus slabThickness coilWeight slabLength slabNum coilNum id link_Event(cond:"{_and:[{processNum:{_eq:\"FCE\"}},{eventTag:{_eq:\"in\"}}]}",authInfo:"",order:"") { timestamp device eventTag processNum coilNum }}}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>link_Event,processNum,FCE,eventTag,in</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT `timestamp`,eventTag,processNum,device,coilNum from Event_local el 
+where `timestamp` &lt; '2022-01-02 08:00:00.000' or `timestamp` &gt;= '2022-01-03 08:05:34.000' order by `timestamp` ASC;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+			  Event(cond:"{_or:[{timestamp:{_lt:\"2022-01-02 08:00:00.000\"}},{timestamp:{_gte:\"2022-01-03 08:05:34.000\"}}]}", authInfo:"", order:"timestamp ASC")
 			  {
-				timestamp
+		                        timestamp
 				eventTag
 				processNum
-				device
+                                                device
 				coilNum
 			  }
 			}</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>ansteel-function-test-17</t>
+  </si>
+  <si>
+    <t>Setting</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">{ 
+  Setting(cond:"{_and:[{coilNum:{_eq:\"P011C00800\"}},{processNum:{_eq:\"R\"}}]}", authInfo:"", order:"value ASC")
+  {
+    coilNum
+    processNum
+    timestamp
+    value
+    sensorId
+    id
+  }
+} </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>chdb</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>SELECT `timestamp`,eventTag,processNum,device,coilNum from Event_local el WHERE coilNum IN ('P011N00700','P011C10400','P011N00300','P011C05000');</t>
+    <t>SELECT * from Setting s WHERE coilNum = 'P011C00800' and processNum ='R' ORDER BY value ASC;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Successfully</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取钢卷所在区域下设置condition(_eq and)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+			  Event(cond:"{_and:[{timestamp:{_lt:\"2022-01-02 08:21:00.000\"}},{timestamp:{_gte:\"2022-01-02 08:20:57.000\"}}]}", authInfo:"", order:"timestamp ASC")
+			  {
+		                        timestamp
+				eventTag
+				processNum
+                                                device
+				coilNum
+			  }
+			}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT `timestamp`,eventTag,processNum,device,coilNum from Event_local el 
+where `timestamp` &gt;= '2022-01-02 08:20:57.000' and `timestamp` &lt; '2022-01-02 08:21:00.000' order by `timestamp` ASC;</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -443,31 +596,31 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -810,27 +963,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13585E94-2A3C-423F-8526-0CA62361FED2}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="59.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="71" style="1" customWidth="1"/>
     <col min="5" max="5" width="14.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="56.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="1"/>
+    <col min="7" max="7" width="56.44140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -844,24 +998,27 @@
         <v>5</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="150" customHeight="1">
+    <row r="2" spans="1:10" ht="150" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>10</v>
@@ -870,27 +1027,28 @@
         <v>9</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G2" s="5">
-        <v>200</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="G2" s="3"/>
       <c r="H2" s="5">
-        <v>100000</v>
-      </c>
-      <c r="I2" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="I2" s="5">
+        <v>100000</v>
+      </c>
+      <c r="J2" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="150" customHeight="1">
+    <row r="3" spans="1:10" ht="150" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>11</v>
@@ -899,275 +1057,422 @@
         <v>9</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G3" s="5">
-        <v>200</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="G3" s="3"/>
       <c r="H3" s="5">
-        <v>100000</v>
-      </c>
-      <c r="I3" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="I3" s="5">
+        <v>100000</v>
+      </c>
+      <c r="J3" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="150" customHeight="1">
+    <row r="4" spans="1:10" ht="150" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="3"/>
+      <c r="H4" s="5">
+        <v>200</v>
+      </c>
+      <c r="I4" s="5">
+        <v>100000</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="150" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="3"/>
+      <c r="H5" s="5">
+        <v>200</v>
+      </c>
+      <c r="I5" s="5">
+        <v>100000</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="150" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G6" s="3"/>
+      <c r="H6" s="5">
+        <v>200</v>
+      </c>
+      <c r="I6" s="5">
+        <v>100000</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="150" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G4" s="5">
-        <v>200</v>
-      </c>
-      <c r="H4" s="5">
-        <v>100000</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="150" customHeight="1">
-      <c r="A5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G5" s="5">
-        <v>200</v>
-      </c>
-      <c r="H5" s="5">
-        <v>100000</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="150" customHeight="1">
-      <c r="A6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="G6" s="5">
-        <v>200</v>
-      </c>
-      <c r="H6" s="5">
-        <v>100000</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="150" customHeight="1">
-      <c r="A7" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>26</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="5">
-        <v>200</v>
-      </c>
       <c r="H7" s="5">
-        <v>100000</v>
-      </c>
-      <c r="I7" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="I7" s="5">
+        <v>100000</v>
+      </c>
+      <c r="J7" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="150" customHeight="1">
+    <row r="8" spans="1:10" ht="150" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="3"/>
+      <c r="H8" s="5">
+        <v>200</v>
+      </c>
+      <c r="I8" s="5">
+        <v>100000</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="184.8" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" s="4" t="s">
+      <c r="E9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H9" s="1">
+        <v>200</v>
+      </c>
+      <c r="I9" s="1">
+        <v>100000</v>
+      </c>
+      <c r="J9" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="G8" s="5">
-        <v>200</v>
-      </c>
-      <c r="H8" s="5">
-        <v>100000</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="150" customHeight="1">
-      <c r="A9" s="3" t="s">
+    </row>
+    <row r="10" spans="1:10" ht="184.8" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B10" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="E10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="H10" s="1">
+        <v>200</v>
+      </c>
+      <c r="I10" s="1">
+        <v>100000</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="330" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F9" s="3" t="s">
+      <c r="B11" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G9" s="5">
-        <v>200</v>
-      </c>
-      <c r="H9" s="5">
-        <v>100000</v>
-      </c>
-      <c r="I9" s="5" t="s">
+      <c r="D11" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" ht="150" customHeight="1">
-      <c r="A10" s="3" t="s">
+      <c r="H11" s="1">
+        <v>200</v>
+      </c>
+      <c r="I11" s="1">
+        <v>100000</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" customFormat="1" ht="158.4" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B12" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D10" s="3" t="s">
+      <c r="D12" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F10" s="3" t="s">
+      <c r="F12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1">
+        <v>200</v>
+      </c>
+      <c r="I12" s="1">
+        <v>100000</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="132" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="G10" s="5">
-        <v>200</v>
-      </c>
-      <c r="H10" s="5">
-        <v>100000</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="150" customHeight="1">
-      <c r="A11" s="3" t="s">
+      <c r="F13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H13" s="1">
+        <v>200</v>
+      </c>
+      <c r="I13" s="1">
+        <v>100000</v>
+      </c>
+      <c r="J13" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C11" s="4" t="s">
+    </row>
+    <row r="14" spans="1:10" ht="158.4" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="G11" s="5">
-        <v>200</v>
-      </c>
-      <c r="H11" s="5">
-        <v>100000</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="150" customHeight="1">
-      <c r="A12" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E12" s="3" t="s">
+      <c r="B14" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H14" s="1">
+        <v>200</v>
+      </c>
+      <c r="I14" s="1">
+        <v>100000</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="158.4" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="B15" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H15" s="1">
+        <v>200</v>
+      </c>
+      <c r="I15" s="1">
+        <v>100000</v>
+      </c>
+      <c r="J15" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="G12" s="5">
-        <v>200</v>
-      </c>
-      <c r="H12" s="5">
-        <v>100000</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>48</v>
+    </row>
+    <row r="16" spans="1:10" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H16" s="1">
+        <v>200</v>
+      </c>
+      <c r="I16" s="1">
+        <v>100000</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="158.4" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H17" s="1">
+        <v>200</v>
+      </c>
+      <c r="I17" s="1">
+        <v>100000</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update test cases for smart space property
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/ansteel-api-engine-test-data.xlsx
+++ b/src/main/resources/test-data-xls/ansteel-api-engine-test-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA0F9DD8-B4E3-4447-B917-6E2FEF07F8CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{258FCCBC-762F-406C-BE2F-547DEC51F72D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1066,8 +1066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13585E94-2A3C-423F-8526-0CA62361FED2}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8"/>
@@ -1324,7 +1324,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8"/>

</xml_diff>

<commit_message>
Add test cases for multiple data sources
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/ansteel-api-engine-test-data.xlsx
+++ b/src/main/resources/test-data-xls/ansteel-api-engine-test-data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{258FCCBC-762F-406C-BE2F-547DEC51F72D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01C97477-C82D-4B15-907E-EF90AE9C1A6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="96">
   <si>
     <t>description</t>
   </si>
@@ -433,23 +433,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>{
-  Coil(cond:"{coilStatus:{_eq:\"true\"}}", authInfo:"", order:"")
-  {
-    coilNum 
-    coilStatus 
-    coilWeight 
-    steelKind 
-    steelGrade 
-    slabLength 
-    slabNum 
-    slabThickness 
-    slabWidth 
-  }
-}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>SELECT coil_no as coilNum, coil_status as coilStatus, coil_weight as coilWeight, steel_kind as steelKind, steel_grade as steelGrade,
 slab_length as slabLength, slab_num as slabNum, slab_thickness as slabThickness, slab_width as slabWidth FROM public.steel_coil where coil_status = true;</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -467,23 +450,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>{
-  Coil(cond:"{coilStatus:{_eq:\"true\"}}", authInfo:"", order:"coilNum ASC")
-  {
-    coilNum 
-    coilStatus 
-    coilWeight 
-    steelKind 
-    steelGrade 
-    slabLength 
-    slabNum 
-    slabThickness 
-    slabWidth 
-  }
-}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>SELECT coil_no as coilNum, coil_status as coilStatus, coil_weight as coilWeight, steel_kind as steelKind, steel_grade as steelGrade,
 slab_length as slabLength, slab_num as slabNum, slab_thickness as slabThickness, slab_width as slabWidth FROM public.steel_coil where coil_status = true order by coil_no ASC;</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -499,6 +465,88 @@
   <si>
     <t>CoilConnection-&gt;edges</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT coil_no as coilNum, coil_status as coilStatus, coil_weight as coilWeight, steel_kind as steelKind, steel_grade as steelGrade,
+slab_length as slabLength, slab_num as slabNum, slab_thickness as slabThickness, slab_width as slabWidth FROM public.steel_coil where coil_status = true order by coil_no ASC limit 20;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>生成节奏监控 获取钢卷Event condition(_in)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Event</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>chdb</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ansteel-function-test-13</t>
+  </si>
+  <si>
+    <t>生成节奏监控 获取钢卷Event condition(_like)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>生成节奏监控 按时间获取Event condition(_and)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>按时间获取Event condition(_or)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>温度仿真 获取正在生产的钢卷对象 condition(_eq and)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  {Coil(cond:"{coilStatus:{_eq:false}}",authInfo:"",order:"") {steelKind steelGrade slabWidth coilStatus slabThickness coilWeight slabLength slabNum coilNum id link_Event(cond:"{_and:[{processNum:{_eq:\"FCE\"}},{eventTag:{_eq:\"in\"}}]}",authInfo:"",order:"") { timestamp device eventTag processNum coilNum }}}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>link_Event,processNum,FCE,eventTag,in</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取钢卷所在区域下设置condition(_eq and)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Setting</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">{ 
+  Setting(cond:"{_and:[{coilNum:{_eq:\"P011C00800\"}},{processNum:{_eq:\"R\"}}]}", authInfo:"", order:"value ASC")
+  {
+    coilNum
+    processNum
+    timestamp
+    value
+    sensorId
+    id
+  }
+} </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT * from Setting s WHERE coilNum = 'P011C00800' and processNum ='R' ORDER BY value ASC;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>nestedEntityWithCondition</t>
+  </si>
+  <si>
+    <t>ansteel-function-test-11</t>
+  </si>
+  <si>
+    <t>ansteel-function-test-12</t>
+  </si>
+  <si>
+    <t>SELECT `timestamp`,eventTag,processNum,device,coilNum from Event_local el WHERE coilNum IN ('N1234567890') order by `timestamp` ASC;</t>
   </si>
   <si>
     <t>{
@@ -525,166 +573,97 @@
     }
   }
 }</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SELECT coil_no as coilNum, coil_status as coilStatus, coil_weight as coilWeight, steel_kind as steelKind, steel_grade as steelGrade,
-slab_length as slabLength, slab_num as slabNum, slab_thickness as slabThickness, slab_width as slabWidth FROM public.steel_coil where coil_status = true order by coil_no ASC limit 20;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ansteel-function-test-11</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>生成节奏监控 获取钢卷Event condition(_in)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Event</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">			{
-			  Event(cond:"{coilNum:{_in:[\"P011N00700\",\"P011C10400\",\"P011N00300\",\"P011C05000\"]}}", authInfo:"", order:"timestamp ASC")
-			  {
-				timestamp
-				eventTag
-				processNum
-				device
-				coilNum
-			  }
-			}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>chdb</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SELECT `timestamp`,eventTag,processNum,device,coilNum from Event_local el WHERE coilNum IN ('P011N00700','P011C10400','P011N00300','P011C05000') order by `timestamp` ASC;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ansteel-function-test-13</t>
-  </si>
-  <si>
-    <t>生成节奏监控 获取钢卷Event condition(_like)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">	 {
-			  Event(cond:"{coilNum:{_like: \"%P010N00%\"}}", order:"timestamp ASC")
-			  {
-				timestamp
-				eventTag
-				processNum
-                                                device
-				coilNum
-			  }
-			}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SELECT `timestamp`,eventTag,processNum,device,coilNum from Event_local el WHERE coilNum LIKE '%P010N00%' order by `timestamp` ASC;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ansteel-function-test-14</t>
-  </si>
-  <si>
-    <t>生成节奏监控 按时间获取Event condition(_and)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>{ 
+  Event(cond:"{coilNum:{_in:[\"N1234567890\"]}}", authInfo:"",order:"timestamp ASC") 
+  { 
+    timestamp
+    eventTag
+    processNum
+    device
+    coilNum
+  }
+}</t>
+  </si>
+  <si>
+    <t>{ 
+  Event(cond:"{coilNum:{_like: \"%1234567890%\"}}", authInfo:"",order:"timestamp ASC") 
+  { 
+    timestamp
+    eventTag
+    processNum
+    device
+    coilNum
+  }
+}</t>
   </si>
   <si>
     <t>{
-			  Event(cond:"{_and:[{timestamp:{_lt:\"2022-01-02 08:21:00.000\"}},{timestamp:{_gte:\"2022-01-02 08:20:57.000\"}}]}", authInfo:"", order:"timestamp ASC")
-			  {
-		                        timestamp
-				eventTag
-				processNum
-                                                device
-				coilNum
-			  }
-			}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+  Coil(cond:"{coilStatus:{_eq:\"true\"}}", authInfo:"", order:"")
+  {
+    coilNum 
+    coilStatus 
+    coilWeight 
+    steelKind 
+    steelGrade 
+    slabLength 
+    slabNum 
+    slabThickness 
+    slabWidth 
+  }
+}</t>
+  </si>
+  <si>
+    <t>{
+  Coil(cond:"{coilStatus:{_eq:\"true\"}}", authInfo:"", order:"coilNum ASC")
+  {
+    coilNum 
+    coilStatus 
+    coilWeight 
+    steelKind 
+    steelGrade 
+    slabLength 
+    slabNum 
+    slabThickness 
+    slabWidth 
+  }
+}</t>
+  </si>
+  <si>
+    <t>SELECT `timestamp`,eventTag,processNum,device,coilNum from Event_local el WHERE coilNum LIKE '%1234567890%' order by `timestamp` ASC;</t>
+  </si>
+  <si>
+    <t>{ 
+  Event(cond:"{_and:[{timestamp:{_gt:\"2022-08-09 16:15:00.000\"}},{timestamp:{_lt:\"2022-08-09 16:15:59.000\"}}]}", authInfo:"",order:"timestamp ASC") 
+  { 
+    timestamp
+    eventTag
+    processNum
+    device
+    coilNum
+  }
+}</t>
   </si>
   <si>
     <t>SELECT `timestamp`,eventTag,processNum,device,coilNum from Event_local el 
-where `timestamp` &gt;= '2022-01-02 08:20:57.000' and `timestamp` &lt; '2022-01-02 08:21:00.000' order by `timestamp` ASC;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ansteel-function-test-15</t>
-  </si>
-  <si>
-    <t>按时间获取Event condition(_or)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>{
-			  Event(cond:"{_or:[{timestamp:{_lt:\"2022-01-02 08:00:00.000\"}},{timestamp:{_gte:\"2022-01-03 08:05:34.000\"}}]}", authInfo:"", order:"timestamp ASC")
-			  {
-		                        timestamp
-				eventTag
-				processNum
-                                                device
-				coilNum
-			  }
-			}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+where `timestamp` &gt;= '2022-08-09 16:15:00.000' and `timestamp` &lt; '2022-08-09 16:15:59.000' order by `timestamp` ASC;</t>
   </si>
   <si>
     <t>SELECT `timestamp`,eventTag,processNum,device,coilNum from Event_local el 
 where `timestamp` &lt; '2022-01-02 08:00:00.000' or `timestamp` &gt;= '2022-01-03 08:05:34.000' order by `timestamp` ASC;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ansteel-function-test-16</t>
-  </si>
-  <si>
-    <t>温度仿真 获取正在生产的钢卷对象 condition(_eq and)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">  {Coil(cond:"{coilStatus:{_eq:false}}",authInfo:"",order:"") {steelKind steelGrade slabWidth coilStatus slabThickness coilWeight slabLength slabNum coilNum id link_Event(cond:"{_and:[{processNum:{_eq:\"FCE\"}},{eventTag:{_eq:\"in\"}}]}",authInfo:"",order:"") { timestamp device eventTag processNum coilNum }}}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>link_Event,processNum,FCE,eventTag,in</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ansteel-function-test-17</t>
-  </si>
-  <si>
-    <t>获取钢卷所在区域下设置condition(_eq and)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Setting</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">{ 
-  Setting(cond:"{_and:[{coilNum:{_eq:\"P011C00800\"}},{processNum:{_eq:\"R\"}}]}", authInfo:"", order:"value ASC")
-  {
+  </si>
+  <si>
+    <t>{ 
+  Event(cond:"{_or:[{timestamp:{_lt:\"2022-01-02 08:00:00.000\"}},{timestamp:{_gte:\"2022-01-03 08:05:34.000\"}}]}", authInfo:"",order:"timestamp ASC") 
+  { 
+    timestamp
+    eventTag
+    processNum
+    device
     coilNum
-    processNum
-    timestamp
-    value
-    sensorId
-    id
   }
-} </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SELECT * from Setting s WHERE coilNum = 'P011C00800' and processNum ='R' ORDER BY value ASC;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>nestedEntityWithCondition</t>
+}</t>
   </si>
 </sst>
 </file>
@@ -1066,8 +1045,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13585E94-2A3C-423F-8526-0CA62361FED2}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8"/>
@@ -1323,7 +1302,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AA0CCED-E1F8-459A-9BA8-92AA389402E6}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -1362,7 +1341,7 @@
         <v>7</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>2</v>
@@ -1490,7 +1469,7 @@
     </row>
     <row r="6" spans="1:10" ht="150" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>57</v>
@@ -1499,13 +1478,13 @@
         <v>58</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>32</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="5">
@@ -1515,27 +1494,27 @@
         <v>100000</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="150" customHeight="1">
       <c r="A7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>62</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>63</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>58</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>64</v>
+        <v>90</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>32</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="5">
@@ -1545,27 +1524,27 @@
         <v>100000</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="150" customHeight="1">
       <c r="A8" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>68</v>
-      </c>
       <c r="D8" s="3" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>32</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="5">
@@ -1575,27 +1554,27 @@
         <v>100000</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="150" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="5">
@@ -1605,27 +1584,27 @@
         <v>100000</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="150" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="5">
@@ -1635,27 +1614,27 @@
         <v>100000</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="150" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="5">
@@ -1665,27 +1644,27 @@
         <v>100000</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="150" customHeight="1">
       <c r="A12" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="5">
@@ -1695,26 +1674,26 @@
         <v>100000</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="150" customHeight="1">
       <c r="A13" s="3" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>58</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="H13" s="5">
         <v>200</v>
@@ -1723,27 +1702,27 @@
         <v>100000</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="150" customHeight="1">
       <c r="A14" s="3" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="5">
@@ -1753,7 +1732,7 @@
         <v>100000</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>